<commit_message>
Add finished lab3 and lab4 part 1
</commit_message>
<xml_diff>
--- a/Lab3/Part3TruthTable.xlsx
+++ b/Lab3/Part3TruthTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,25 +476,25 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -511,25 +511,25 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -546,25 +546,25 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -581,25 +581,25 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -616,25 +616,25 @@
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -651,25 +651,25 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -686,25 +686,25 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -721,25 +721,25 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -756,25 +756,25 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -791,25 +791,25 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -826,25 +826,25 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -861,25 +861,25 @@
         <v>1</v>
       </c>
       <c r="E13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -896,25 +896,25 @@
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -931,25 +931,25 @@
         <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -966,25 +966,25 @@
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1001,25 +1001,25 @@
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>